<commit_message>
start working with Census API
</commit_message>
<xml_diff>
--- a/OriginalMaterials/Table 1.xlsx
+++ b/OriginalMaterials/Table 1.xlsx
@@ -1,31 +1,41 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24430"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Dropbox\papers\2017\Baccini Weymouth 2017\Draft\APSR\R&amp;R Draft\US level data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Zagreb\Downloads\Docs\Research\ReplicationPaper\OriginalMaterials\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{74BA2845-4744-4B90-9428-0FD0B7C2F6C5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="14160" windowHeight="12030" activeTab="1"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="employment_race" sheetId="1" r:id="rId1"/>
     <sheet name="layoffs_race" sheetId="2" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:Single"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:CNMTM"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="78" uniqueCount="41">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="79" uniqueCount="41">
   <si>
     <t>White Alone</t>
   </si>
@@ -153,7 +163,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="1">
     <numFmt numFmtId="164" formatCode="0.000"/>
   </numFmts>
@@ -475,11 +485,11 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="K36" sqref="K36"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1280,31 +1290,31 @@
         <v>38</v>
       </c>
       <c r="B36" s="3">
-        <f>B34/$B$35</f>
+        <f t="shared" ref="B36:H36" si="1">B34/$B$35</f>
         <v>0.81362585107025764</v>
       </c>
       <c r="C36" s="3">
-        <f>C34/$B$35</f>
+        <f t="shared" si="1"/>
         <v>9.8529747977398233E-2</v>
       </c>
       <c r="D36" s="3">
-        <f>D34/$B$35</f>
+        <f t="shared" si="1"/>
         <v>8.7636698777184309E-3</v>
       </c>
       <c r="E36" s="3">
-        <f>E34/$B$35</f>
+        <f t="shared" si="1"/>
         <v>6.3600994082030959E-2</v>
       </c>
       <c r="F36" s="3">
-        <f>F34/$B$35</f>
+        <f t="shared" si="1"/>
         <v>2.2242401316933829E-3</v>
       </c>
       <c r="G36" s="3">
-        <f>G34/$B$35</f>
+        <f t="shared" si="1"/>
         <v>1.3255496860901323E-2</v>
       </c>
       <c r="H36" s="3">
-        <f>H34/$B$35</f>
+        <f t="shared" si="1"/>
         <v>0.14645181999751028</v>
       </c>
     </row>
@@ -1314,11 +1324,11 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A1:H35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="L28" sqref="L28"/>
+      <selection activeCell="H1" sqref="H1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -1345,6 +1355,9 @@
       <c r="G1" s="1" t="s">
         <v>5</v>
       </c>
+      <c r="H1" s="1" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">

</xml_diff>